<commit_message>
actually added ICA this time
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/CST-247-RS-SprintBurnDownTemplate-3Weeks (1).xlsx
+++ b/Documentation/Scrum/CST-247-RS-SprintBurnDownTemplate-3Weeks (1).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gcu.edu\home\HomeDrive\andrew.silver\profile\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ali\Documents\cst247\Documentation\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -72,11 +72,6 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>Project Title:
-Release #:
-Sprint #:</t>
-  </si>
-  <si>
     <t>User Story ID</t>
   </si>
   <si>
@@ -86,27 +81,6 @@
     <t>Team Member</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
     <t>Task 8</t>
   </si>
   <si>
@@ -174,12 +148,41 @@
   </si>
   <si>
     <t>After each Daily Standup each Team Member should review the Burn Down Chart to ensure your Sprint will be delivered on time</t>
+  </si>
+  <si>
+    <t>Project Title: Minesweeper
+Release #: 1.0.0
+Sprint #: 1</t>
+  </si>
+  <si>
+    <t>Implement Register Controller</t>
+  </si>
+  <si>
+    <t>Ali Cooper</t>
+  </si>
+  <si>
+    <t>Implement Registration Database integration</t>
+  </si>
+  <si>
+    <t>As a user I would like to be able to register an account to login to the site</t>
+  </si>
+  <si>
+    <t>As a user I need to login in order to play minesweeper</t>
+  </si>
+  <si>
+    <t>Implement Register View with forms</t>
+  </si>
+  <si>
+    <t>Implement Login Controller</t>
+  </si>
+  <si>
+    <t>Implement Login View &amp; Associated Forms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +324,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -350,7 +353,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -382,7 +384,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -465,6 +466,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94D7-455D-AB54-5A94C0B1FAE3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -489,7 +495,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -572,6 +577,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-94D7-455D-AB54-5A94C0B1FAE3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -622,7 +632,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -654,7 +663,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1054,7 +1069,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C11" sqref="B8:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1082,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1099,16 +1114,16 @@
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -1146,22 +1161,22 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F4" s="4">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
@@ -1196,27 +1211,27 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10"/>
       <c r="D5" s="9" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F5" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
       </c>
       <c r="H5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4">
         <v>0</v>
@@ -1228,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N5" s="4">
         <v>0</v>
@@ -1242,27 +1257,27 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10"/>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
       </c>
       <c r="H6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="4">
         <v>0</v>
@@ -1292,45 +1307,19 @@
       <c r="A7" s="1"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0</v>
-      </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
@@ -1340,16 +1329,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -1361,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4">
         <v>0</v>
@@ -1384,15 +1373,15 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -1410,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -1434,12 +1423,8 @@
       <c r="A10" s="1"/>
       <c r="B10" s="7"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="4">
         <v>0</v>
       </c>
@@ -1482,13 +1467,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -1526,19 +1511,17 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="7">
         <v>4</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -1582,13 +1565,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
@@ -1636,43 +1619,43 @@
       <c r="E14" s="12"/>
       <c r="F14" s="4">
         <f>SUM(F4:F13)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G14" s="4">
         <f>F14-$F$14/10</f>
-        <v>27</v>
+        <v>4.5</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14:P14" si="0">G14-$F$14/10</f>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3.5</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2.5</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" si="0"/>
@@ -1691,47 +1674,47 @@
       <c r="E15" s="12"/>
       <c r="F15" s="4">
         <f>SUM(F4:F13)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" ref="G15:P15" si="1">F15 - SUM(G4:G13)</f>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>-1</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>-2</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>-7</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>-7</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>-9</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-14</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-14</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2207,74 +2190,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2343,30 +2326,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Course Development" ma:contentTypeID="0x010100A30BC5E90BED914E81F4B67CDEADBEEF0072B4D5296E9CCD41A4B955E8BC4A98B900B6D41DF35BCF664B888FA24C3105B583" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new Course Development document." ma:contentTypeScope="" ma:versionID="9dd9ed6e3bbe7b4f5b00c4ab3cb49488">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="30a82cfc-8d0b-455e-b705-4035c60ff9fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f302115a5f8a1b15560b600ae7cd187" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2595,6 +2554,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2649,30 +2632,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B20B8EA-C8C4-49B1-8280-945BA6550F81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D14C1044-F523-4937-BF47-727729F19EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26BAEAB1-84F8-4623-9116-5B777FA60CDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2687,6 +2646,30 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D14C1044-F523-4937-BF47-727729F19EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B20B8EA-C8C4-49B1-8280-945BA6550F81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>